<commit_message>
Exercises for Feb 9, 2023
</commit_message>
<xml_diff>
--- a/data/us_elections.xlsx
+++ b/data/us_elections.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,574 +434,601 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>State</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Official/Unofficial</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Total Ballots Counted (Estimate)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Vote for Highest Office (President)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>VEP Turnout Rate</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Voting-Eligible Population (VEP)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Voting-Age Population (VAP)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>% Non-citizen</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Prison</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Probation</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Parole</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Total Ineligible Felon</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Overseas Eligible</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>State Abv</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
         <v>158835004</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>0.664</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>239247182</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>257605088</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>7.8%</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>1461074</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1962811</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>616440</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>3294457</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>4971025</v>
       </c>
-      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Alabama</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>https://www2.alabamavotes.gov/electionnight/statewideResultsByContest.aspx?ecode=1001090</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>2306587</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>2,297,295</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.626</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>3683055</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>3837540</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>2.3%</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>25898</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>50997</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>10266</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>67782</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
         <is>
           <t>AL</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Alaska</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>https://www.elections.alaska.gov/results/20GENR/index.php</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
         <v>367000</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
         <v>0.698</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>525568</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>551117</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>3.4%</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>4293</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>2074</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>1348</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>6927</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
         <is>
           <t>AK</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Arizona</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>https://results.arizona.vote/#/featured/18/0</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
         <v>3400000</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
         <v>0.655</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>5189000</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>5798473</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>8.9%</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>38520</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>76844</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>7536</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>93699</v>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
         <is>
           <t>AZ</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Arkansas</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>https://results.enr.clarityelections.com/AR/106124/web.264614/#/summary</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1212030</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>1,206,697</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.555</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>2182375</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>2331171</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>3.6%</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>17510</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>36719</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>24698</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>64974</v>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
         <is>
           <t>AR</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>California</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>https://electionresults.sos.ca.gov/</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>16800000</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
         <v>0.647</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>25962648</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>30783255</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>15.0%</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>104730</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
       <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
         <v>102586</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>207316</v>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Colorado</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>https://results.enr.clarityelections.com/CO/105975/web.264614/#/summary</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="n">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
         <v>3295000</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
         <v>0.764</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>4313054</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>4595504</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>5.7%</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>18905</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>18905</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
         <is>
           <t>CO</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Connecticut</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="n">
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
         <v>1850000</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
         <v>0.711</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>2603327</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>2839560</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>7.7%</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>13268</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
       <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>4452</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>17720</v>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
         <is>
           <t>CT</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Delaware</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>https://elections.delaware.gov/results/html/index.shtml?electionId=GE2020</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>507805</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>502,392</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>0.705</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>720531</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>780822</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>5.8%</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>5874</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>14176</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>350</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>15013</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr">
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
         <is>
           <t>DE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>District of Columbia</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>https://electionresults.dcboe.org/election_results/2020-General-Election</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
         <v>350000</v>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
         <v>0.647</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>540685</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>582065</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>7.1%</t>
         </is>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
@@ -1011,568 +1038,601 @@
       <c r="M11" t="n">
         <v>0</v>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
         <is>
           <t>DC</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Florida</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>https://floridaelectionwatch.gov/CountyReportingStatus</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="n">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
         <v>11150000</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
         <v>0.7170000000000001</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>15551739</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>17543341</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>10.1%</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>91674</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>205033</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>4345</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>223139</v>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Georgia</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>https://results.enr.clarityelections.com/GA/105369/web.264614/</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
         <v>5025000</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
         <v>0.6809999999999999</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>7383562</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>8255108</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>6.6%</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>50930</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>416771</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>20426</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>329754</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
         <is>
           <t>GA</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>https://elections.hawaii.gov/wp-content/results/histatewide.pdf</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>579165</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>573,854</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>0.575</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>1007920</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>1114466</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>9.1%</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>5007</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
         <v>5007</v>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
         <is>
           <t>HI</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>https://www.livevoterturnout.com/Idaho/LiveResults/1/en/Index_113.html</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>875000</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>867,258</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.677</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1292701</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>1384683</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>4.1%</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>8378</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>34392</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>5267</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>34968</v>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Illinois</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
         <v>6100000</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
         <v>0.6759999999999999</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>9027082</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>9832749</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>7.8%</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>38464</v>
       </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
         <v>38464</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
         <is>
           <t>IL</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Indiana</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>https://enr.indianavoters.in.gov/site/index.html</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
         <v>3070000</v>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>0.614</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>5000007</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>5214546</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>3.6%</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>26302</v>
       </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
         <v>26302</v>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
         <is>
           <t>IN</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Iowa</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>https://electionresults.iowa.gov/IA/106279/web.264614/#/summary</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="n">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="n">
         <v>1825000</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
         <v>0.7859999999999999</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>2321131</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>2439743</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>3.5%</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>9216</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>29137</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>6652</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>33933</v>
       </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
         <is>
           <t>IA</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Kansas</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>https://ent.sos.ks.gov/kssos_ent.html</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>1340000</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>1,333,513</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>0.642</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>2087946</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>2223238</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>4.9%</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>9882</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>16455</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>5438</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>25522</v>
       </c>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr">
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr">
         <is>
           <t>KS</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Kentucky</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>https://results.enr.clarityelections.com/KY/106379/web.264614/#/summary</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>2150951</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>2,134,993</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>0.649</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3312250</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>3479257</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>2.8%</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>23280</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>46967</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>15881</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>68281</v>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
         <is>
           <t>KY</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Louisiana</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>https://voterportal.sos.la.gov/graphical</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>2155000</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>2,147,395</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.639</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>3373932</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>3557594</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>2.8%</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>32267</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>35025</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>29321</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>83304</v>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
         <is>
           <t>LA</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
         <v>860000</v>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
         <v>0.792</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>1085285</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>1104489</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>1.7%</t>
         </is>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>
@@ -1582,1359 +1642,1437 @@
       <c r="M22" t="n">
         <v>0</v>
       </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
         <is>
           <t>ME</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>https://elections.maryland.gov/county_status_page_root.html</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
         <v>3050000</v>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
         <v>0.7070000000000001</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>4313416</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>4729400</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>8.4%</t>
         </is>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>18165</v>
       </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
       <c r="L23" t="n">
         <v>0</v>
       </c>
       <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
         <v>18165</v>
       </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
         <is>
           <t>MD</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>Massachusetts</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
         <v>3725000</v>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
         <v>0.7340000000000001</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>5072901</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>5566452</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>8.7%</t>
         </is>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>7772</v>
       </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
       <c r="L24" t="n">
         <v>0</v>
       </c>
       <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
         <v>7772</v>
       </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Michigan</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>https://mielections.us/election/results/2020GEN_CENR.html</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>5559186</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>5,519,348</t>
         </is>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>0.736</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>7550147</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>7870864</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>3.6%</t>
         </is>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>38183</v>
       </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
       <c r="L25" t="n">
         <v>0</v>
       </c>
       <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
         <v>38183</v>
       </c>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
         <is>
           <t>MI</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Minnesota</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>https://electionresults.sos.state.mn.us/20201103</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>3290000</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>3,278,405</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>0.799</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>4118462</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>4378737</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>4.1%</t>
         </is>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>9712</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>100076</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>7381</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>79140</v>
       </c>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr">
         <is>
           <t>MN</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Mississippi</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="n">
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="n">
         <v>1330000</v>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="n">
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
         <v>0.604</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>2201950</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>2279412</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>1.4%</t>
         </is>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>19244</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>27294</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>9866</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>46032</v>
       </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr">
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
         <is>
           <t>MS</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Missouri</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>https://enr.sos.mo.gov/</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>3050000</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>3,012,436</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>0.6629999999999999</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>4603060</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>4794796</v>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>2.4%</t>
         </is>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>30148</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>43871</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>19251</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>76599</v>
       </c>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr">
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
         <is>
           <t>MO</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Montana</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>https://electionresults.mt.gov/</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>612055</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>603,635</t>
         </is>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>0.731</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>837298</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>851663</v>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>1.2%</t>
         </is>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>3754</v>
       </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
       <c r="L29" t="n">
         <v>0</v>
       </c>
       <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
         <v>3754</v>
       </c>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr">
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
         <is>
           <t>MT</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Nebraska</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>https://electionresults.nebraska.gov/</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>948852</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>935,232</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>0.6859999999999999</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>1383551</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>1469878</v>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>4.8%</t>
         </is>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>5263</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>14894</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>958</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>15455</v>
       </c>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr">
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr">
         <is>
           <t>NE</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Nevada</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="n">
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
         <v>1370000</v>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="n">
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="n">
         <v>0.636</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>2153915</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>2450946</v>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>11.6%</t>
         </is>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>12399</v>
       </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
       <c r="L31" t="n">
         <v>0</v>
       </c>
       <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
         <v>12399</v>
       </c>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr">
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
         <is>
           <t>NV</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>New Hampshire</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>https://sos.nh.gov/elections/elections/election-results/2020/general-election/</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>814092</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>803,833</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.754</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>1079434</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>1115916</v>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>3.0%</t>
         </is>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>2635</v>
       </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
       <c r="L32" t="n">
         <v>0</v>
       </c>
       <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
         <v>2635</v>
       </c>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr">
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
         <is>
           <t>NH</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>New Jersey</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
         <v>4495000</v>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="n">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="n">
         <v>0.73</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>6158999</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>6952008</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>11.1%</t>
         </is>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>18099</v>
       </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
       <c r="L33" t="n">
         <v>0</v>
       </c>
       <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>18099</v>
       </c>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr">
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
         <is>
           <t>NJ</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>New Mexico</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>https://nmresults.azurewebsites.net/Default.aspx</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>923612</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>919,377</t>
         </is>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.61</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>1515355</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>1634037</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>6.2%</t>
         </is>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>6887</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>12090</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>2805</v>
       </c>
-      <c r="M34" t="n">
+      <c r="N34" t="n">
         <v>17188</v>
       </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr">
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
         <is>
           <t>NM</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>New York</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="n">
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
         <v>8930000</v>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="n">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
         <v>0.653</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>13670596</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>15372655</v>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>10.5%</t>
         </is>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>42408</v>
       </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
       <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
         <v>45192</v>
       </c>
-      <c r="M35" t="n">
+      <c r="N35" t="n">
         <v>87600</v>
       </c>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr">
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr">
         <is>
           <t>NY</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>North Carolina</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>https://www.ncsbe.gov/results-data/election-results</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="n">
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
         <v>5600000</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="n">
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="n">
         <v>0.722</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>7759051</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>8328642</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>5.7%</t>
         </is>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>33640</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>80068</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>14215</v>
       </c>
-      <c r="M36" t="n">
+      <c r="N36" t="n">
         <v>97497</v>
       </c>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr">
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
         <is>
           <t>NC</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>North Dakota</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>https://results.sos.nd.gov/Default.aspx?map=Cty</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>365000</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>357,916</t>
         </is>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>0.6459999999999999</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>565143</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>584610</v>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>3.0%</t>
         </is>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>1679</v>
       </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
       <c r="L37" t="n">
         <v>0</v>
       </c>
       <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
         <v>1679</v>
       </c>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr">
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr">
         <is>
           <t>ND</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>https://liveresults.ohiosos.gov/</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="n">
         <v>6100000</v>
       </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="n">
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
         <v>0.6890000000000001</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>8859167</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>9144626</v>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>2.6%</t>
         </is>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>49892</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
       <c r="L38" t="n">
         <v>0</v>
       </c>
       <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
         <v>49892</v>
       </c>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr">
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr">
         <is>
           <t>OH</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>Oklahoma</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>https://www.ok.gov/elections/Election_Info/2020_November_General_Election.html</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>OFFICIAL</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>1565000</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>1,560,699</t>
         </is>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>0.55</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>2845835</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>3031792</v>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t>4.3%</t>
         </is>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>27558</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>41562</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>1780</v>
       </c>
-      <c r="M39" t="n">
+      <c r="N39" t="n">
         <v>55106</v>
       </c>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr">
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Oregon</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>https://results.oregonvotes.gov/Default.aspx</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>2404642</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>2,334,666</t>
         </is>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.752</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>3196425</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>3405863</v>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="J40" t="inlineStr">
         <is>
           <t>5.7%</t>
         </is>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>13795</v>
       </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
       <c r="L40" t="n">
         <v>0</v>
       </c>
       <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
         <v>13795</v>
       </c>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr">
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Pennsylvania</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>https://www.electionreturns.pa.gov/</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="n">
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="n">
         <v>6900000</v>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="n">
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="n">
         <v>0.705</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>9781976</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>10186170</v>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>3.5%</t>
         </is>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>44148</v>
       </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
       <c r="L41" t="n">
         <v>0</v>
       </c>
       <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
         <v>44148</v>
       </c>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr">
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
         <is>
           <t>PA</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Rhode Island</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="n">
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
         <v>520000</v>
       </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="n">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="n">
         <v>0.65</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>799642</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>857507</v>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="J42" t="inlineStr">
         <is>
           <t>6.4%</t>
         </is>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>2766</v>
       </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
       <c r="L42" t="n">
         <v>0</v>
       </c>
       <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
         <v>2766</v>
       </c>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr">
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
         <is>
           <t>RI</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>South Carolina</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>https://www.enr-scvotes.org/SC/106502/Web02-state.264691/#/?undefined</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>2532995</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>2,513,314</t>
         </is>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>0.645</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>3926305</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>4116633</v>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>3.6%</t>
         </is>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>18587</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>31975</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>4980</v>
       </c>
-      <c r="M43" t="n">
+      <c r="N43" t="n">
         <v>43392</v>
       </c>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
         <is>
           <t>SC</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>South Dakota</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>http://electionresults.sd.gov/Default.aspx</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>427529</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>422,609</t>
         </is>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>0.66</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>648104</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>675016</v>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr">
         <is>
           <t>2.4%</t>
         </is>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>3867</v>
       </c>
-      <c r="K44" t="n">
+      <c r="L44" t="n">
         <v>5989</v>
       </c>
-      <c r="L44" t="n">
+      <c r="M44" t="n">
         <v>3201</v>
       </c>
-      <c r="M44" t="n">
+      <c r="N44" t="n">
         <v>10781</v>
       </c>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr">
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Tennessee</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>https://elections.tn.gov/results.php</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>3060000</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>3,045,401</t>
         </is>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>0.597</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>5124867</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>5391220</v>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>3.6%</t>
         </is>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>26107</v>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>61253</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
         <v>10842</v>
       </c>
-      <c r="M45" t="n">
+      <c r="N45" t="n">
         <v>74926</v>
       </c>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr">
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
         <is>
           <t>TN</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Texas</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>https://results.texas-election.com/races</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>11300000</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>11,231,799</t>
         </is>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>0.602</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>18784280</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>22058260</v>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>12.6%</t>
         </is>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>154913</v>
       </c>
-      <c r="K46" t="n">
+      <c r="L46" t="n">
         <v>368167</v>
       </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
         <v>109213</v>
       </c>
-      <c r="M46" t="n">
+      <c r="N46" t="n">
         <v>492390</v>
       </c>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr">
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
         <is>
           <t>TX</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Utah</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>https://electionresults.utah.gov/elections/</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="n">
         <v>1450000</v>
       </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="n">
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
         <v>0.662</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>2191487</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>2343384</v>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="J47" t="inlineStr">
         <is>
           <t>6.2%</t>
         </is>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>6287</v>
       </c>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
       <c r="L47" t="n">
         <v>0</v>
       </c>
       <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
         <v>6287</v>
       </c>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr">
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
         <is>
           <t>UT</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>Vermont</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>https://electionresults.vermont.gov/Index.html#/federal</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
         <v>370000</v>
       </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="n">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
         <v>0.74</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>499884</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>511637</v>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>2.3%</t>
         </is>
       </c>
-      <c r="J48" t="n">
-        <v>0</v>
-      </c>
       <c r="K48" t="n">
         <v>0</v>
       </c>
@@ -2944,261 +3082,279 @@
       <c r="M48" t="n">
         <v>0</v>
       </c>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr">
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr">
         <is>
           <t>VT</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>Virginia</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>https://results.elections.virginia.gov/vaelections/2020%20November%20General/Site/Presidential.html</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Unofficial</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>4425000</v>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>4,409,913</t>
         </is>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>0.7140000000000001</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>6196071</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>6727440</v>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>6.8%</t>
         </is>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>35743</v>
       </c>
-      <c r="K49" t="n">
+      <c r="L49" t="n">
         <v>63111</v>
       </c>
-      <c r="L49" t="n">
+      <c r="M49" t="n">
         <v>1860</v>
       </c>
-      <c r="M49" t="n">
+      <c r="N49" t="n">
         <v>76732</v>
       </c>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr">
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr">
         <is>
           <t>VA</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Washington</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>https://results.vote.wa.gov/results/20201103/turnout.html</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="n">
         <v>4100000</v>
       </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="n">
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="n">
         <v>0.754</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>5437844</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>6070046</v>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="J50" t="inlineStr">
         <is>
           <t>9.1%</t>
         </is>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>18777</v>
       </c>
-      <c r="K50" t="n">
+      <c r="L50" t="n">
         <v>76672</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
         <v>12222</v>
       </c>
-      <c r="M50" t="n">
+      <c r="N50" t="n">
         <v>78536</v>
       </c>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr">
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
         <is>
           <t>WA</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>West Virginia</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
         <v>795000</v>
       </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="n">
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="n">
         <v>0.57</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>1394028</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>1422098</v>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>0.9%</t>
         </is>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>6757</v>
       </c>
-      <c r="K51" t="n">
+      <c r="L51" t="n">
         <v>6593</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
         <v>4287</v>
       </c>
-      <c r="M51" t="n">
+      <c r="N51" t="n">
         <v>15132</v>
       </c>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
         <is>
           <t>WV</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>Wisconsin</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
-      <c r="D52" t="n">
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
         <v>3325000</v>
       </c>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="n">
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
         <v>0.7609999999999999</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>4368530</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>4586746</v>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>3.2%</t>
         </is>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>23574</v>
       </c>
-      <c r="K52" t="n">
+      <c r="L52" t="n">
         <v>42909</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
         <v>21015</v>
       </c>
-      <c r="M52" t="n">
+      <c r="N52" t="n">
         <v>71193</v>
       </c>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr">
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
         <is>
           <t>WI</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>Wyoming</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>https://sos.wyo.gov/Elections/Docs/2020/2020GeneralResults.aspx</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>OFFICIAL</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="E53" t="n">
         <v>278503</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>276,765</t>
         </is>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0.6459999999999999</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>431364</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>447915</v>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>2.2%</t>
         </is>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>2488</v>
       </c>
-      <c r="K53" t="n">
+      <c r="L53" t="n">
         <v>5383</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
         <v>934</v>
       </c>
-      <c r="M53" t="n">
+      <c r="N53" t="n">
         <v>6759</v>
       </c>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr">
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr">
         <is>
           <t>WY</t>
         </is>

</xml_diff>